<commit_message>
posted materials after Matlab class
</commit_message>
<xml_diff>
--- a/sample_sheet.xlsx
+++ b/sample_sheet.xlsx
@@ -4,15 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Temperatures" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,10 +387,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E3:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>